<commit_message>
Huge permission systems are huge.
</commit_message>
<xml_diff>
--- a/Discord Groups/Discord Groups - Server/storage template/permissions.xlsx
+++ b/Discord Groups/Discord Groups - Server/storage template/permissions.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\developer\Documents\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\developer\Wee Utilities\Discord Groups\Discord Groups - Server\storage template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="(Guid ID)" sheetId="1" r:id="rId1"/>
+    <sheet name="(Guid ID) - Users" sheetId="1" r:id="rId1"/>
+    <sheet name="(Guild ID) - Roles" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="8">
   <si>
     <t>(Discord User ID)</t>
   </si>
@@ -45,6 +46,9 @@
   </si>
   <si>
     <t>……</t>
+  </si>
+  <si>
+    <t>(Discord Role ID)</t>
   </si>
 </sst>
 </file>
@@ -86,8 +90,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -398,13 +430,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" customWidth="1"/>
@@ -572,4 +604,184 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>